<commit_message>
Mise à jour visuel du planning
</commit_message>
<xml_diff>
--- a/planning_Gabriel_Strano_TPI_2016.xlsx
+++ b/planning_Gabriel_Strano_TPI_2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="0" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="270" yWindow="60" windowWidth="20115" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Activité</t>
   </si>
@@ -61,6 +61,11 @@
   </si>
   <si>
     <t>weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabriel Strano
+IFA-P3A
+Planning TPI </t>
   </si>
 </sst>
 </file>
@@ -70,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +117,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -161,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -387,6 +398,30 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -395,11 +430,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,35 +458,47 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -758,265 +802,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:15" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
+    </row>
+    <row r="2" spans="1:15" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26">
+      <c r="C2" s="20">
         <v>42524</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26">
+      <c r="E2" s="20">
         <v>42526</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="26">
+      <c r="G2" s="20">
         <v>42528</v>
       </c>
-      <c r="H1" s="26">
+      <c r="H2" s="20">
         <v>42529</v>
       </c>
-      <c r="I1" s="26">
+      <c r="I2" s="20">
         <v>42530</v>
       </c>
-      <c r="J1" s="26">
+      <c r="J2" s="20">
         <v>42531</v>
       </c>
-      <c r="K1" s="26">
+      <c r="K2" s="20">
         <v>42532</v>
       </c>
-      <c r="L1" s="26">
+      <c r="L2" s="20">
         <v>42533</v>
       </c>
-      <c r="M1" s="26">
+      <c r="M2" s="20">
         <v>42534</v>
       </c>
-      <c r="N1" s="26">
+      <c r="N2" s="20">
         <v>42535</v>
       </c>
-      <c r="O1" s="29">
+      <c r="O2" s="23">
         <v>42536</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="25" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="25" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="6"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="5"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="6"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="6"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="24"/>
+      <c r="A5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="6"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="15"/>
+      <c r="A8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="6"/>
+      <c r="A9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="17"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="16"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="21"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D2:E11"/>
-    <mergeCell ref="K2:L11"/>
+  <mergeCells count="3">
+    <mergeCell ref="D3:E12"/>
+    <mergeCell ref="K3:L12"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>